<commit_message>
Roté el mapa de la topología. Terrible cambio :) Seccionada la red A (X.25) en A1-A6, asignadas las direcciones y hechas las tablas. Agregadas las redes F y G con sus direcciones. No estoy muy seguro de poner H7-B por ejemplo para indicar la conexión entre el router 7 y el equipo contra el que está conectado en internet, pero las direcciones valen.
</commit_message>
<xml_diff>
--- a/Datos+Redes.xlsx
+++ b/Datos+Redes.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="203">
   <si>
     <t>Nombre</t>
   </si>
@@ -265,13 +265,376 @@
   </si>
   <si>
     <t>10.38.23.92</t>
+  </si>
+  <si>
+    <t>Dirección</t>
+  </si>
+  <si>
+    <t>Máscara</t>
+  </si>
+  <si>
+    <t>Broadcast</t>
+  </si>
+  <si>
+    <t>10.5.1.71</t>
+  </si>
+  <si>
+    <t>10.38.23.252</t>
+  </si>
+  <si>
+    <t>10.38.23.255</t>
+  </si>
+  <si>
+    <t>10.38.23.144</t>
+  </si>
+  <si>
+    <t>255.255.255.0</t>
+  </si>
+  <si>
+    <t>10.38.23.159</t>
+  </si>
+  <si>
+    <t>10.38.23.191</t>
+  </si>
+  <si>
+    <t>157.43.1.248</t>
+  </si>
+  <si>
+    <t>157.43.1.252</t>
+  </si>
+  <si>
+    <t>10.38.23.96</t>
+  </si>
+  <si>
+    <t>10.38.23.248</t>
+  </si>
+  <si>
+    <t>192.168.23.255</t>
+  </si>
+  <si>
+    <t>255.255.255.248</t>
+  </si>
+  <si>
+    <t>255.255.255.192</t>
+  </si>
+  <si>
+    <t>255.255.255.252</t>
+  </si>
+  <si>
+    <t>255.255.255.240</t>
+  </si>
+  <si>
+    <t>255.255.255.128</t>
+  </si>
+  <si>
+    <t>255.255.255.224</t>
+  </si>
+  <si>
+    <t>157.43.1.251</t>
+  </si>
+  <si>
+    <t>157.43.1.255</t>
+  </si>
+  <si>
+    <t>10.38.23.127</t>
+  </si>
+  <si>
+    <t>10.38.23.251</t>
+  </si>
+  <si>
+    <t>10.38.23.143</t>
+  </si>
+  <si>
+    <t>10.38.23.95</t>
+  </si>
+  <si>
+    <t>10.38.1.127</t>
+  </si>
+  <si>
+    <t>10.7.1.255</t>
+  </si>
+  <si>
+    <t>10.38.1.255</t>
+  </si>
+  <si>
+    <t>Máscaras</t>
+  </si>
+  <si>
+    <t>10.5.1.70</t>
+  </si>
+  <si>
+    <t>Primer host</t>
+  </si>
+  <si>
+    <t>Ultimo host</t>
+  </si>
+  <si>
+    <t>10.38.23.1</t>
+  </si>
+  <si>
+    <t>10.38.23.190</t>
+  </si>
+  <si>
+    <t>10.38.23.253</t>
+  </si>
+  <si>
+    <t>10.38.23.145</t>
+  </si>
+  <si>
+    <t>157.43.1.249</t>
+  </si>
+  <si>
+    <t>157.43.1.253</t>
+  </si>
+  <si>
+    <t>10.38.23.97</t>
+  </si>
+  <si>
+    <t>10.38.23.249</t>
+  </si>
+  <si>
+    <t>10.38.23.65</t>
+  </si>
+  <si>
+    <t>10.38.1.1</t>
+  </si>
+  <si>
+    <t>10.38.1.129</t>
+  </si>
+  <si>
+    <t>10.38.23.254</t>
+  </si>
+  <si>
+    <t>10.38.23.158</t>
+  </si>
+  <si>
+    <t>192.168.23.254</t>
+  </si>
+  <si>
+    <t>157.43.1.250</t>
+  </si>
+  <si>
+    <t>157.43.1.254</t>
+  </si>
+  <si>
+    <t>10.38.23.126</t>
+  </si>
+  <si>
+    <t>10.38.23.250</t>
+  </si>
+  <si>
+    <t>10.38.23.142</t>
+  </si>
+  <si>
+    <t>10.38.23.94</t>
+  </si>
+  <si>
+    <t>10.38.1.126</t>
+  </si>
+  <si>
+    <t>10.7.1.254</t>
+  </si>
+  <si>
+    <t>10.38.1.254</t>
+  </si>
+  <si>
+    <t>Host A</t>
+  </si>
+  <si>
+    <t>TelServer</t>
+  </si>
+  <si>
+    <t>Host C</t>
+  </si>
+  <si>
+    <t>FTPServer</t>
+  </si>
+  <si>
+    <t>Host B</t>
+  </si>
+  <si>
+    <t>10.38.23.3</t>
+  </si>
+  <si>
+    <t>10.38.23.2</t>
+  </si>
+  <si>
+    <t>10.38.23.4</t>
+  </si>
+  <si>
+    <t>10.38.23.5</t>
+  </si>
+  <si>
+    <t>10.38.23.98</t>
+  </si>
+  <si>
+    <t>10.38.23.66</t>
+  </si>
+  <si>
+    <t>10.38.23.68</t>
+  </si>
+  <si>
+    <t>10.38.23.67</t>
+  </si>
+  <si>
+    <t>10.38.1.2</t>
+  </si>
+  <si>
+    <t>10.38.1.3</t>
+  </si>
+  <si>
+    <t>10.5.1.64 (X.25)</t>
+  </si>
+  <si>
+    <t>10.4.3.0</t>
+  </si>
+  <si>
+    <t>157.43.1.0 (Internet)</t>
+  </si>
+  <si>
+    <t>.0</t>
+  </si>
+  <si>
+    <t>.16</t>
+  </si>
+  <si>
+    <t>.32</t>
+  </si>
+  <si>
+    <t>.48</t>
+  </si>
+  <si>
+    <t>.64</t>
+  </si>
+  <si>
+    <t>.80</t>
+  </si>
+  <si>
+    <t>.96</t>
+  </si>
+  <si>
+    <t>.112</t>
+  </si>
+  <si>
+    <t>.128</t>
+  </si>
+  <si>
+    <t>.144</t>
+  </si>
+  <si>
+    <t>.160</t>
+  </si>
+  <si>
+    <t>.176</t>
+  </si>
+  <si>
+    <t>.192</t>
+  </si>
+  <si>
+    <t>.208</t>
+  </si>
+  <si>
+    <t>.224</t>
+  </si>
+  <si>
+    <t>.240</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>10.5.1.72</t>
+  </si>
+  <si>
+    <t>10.5.1.76</t>
+  </si>
+  <si>
+    <t>10.5.1.80</t>
+  </si>
+  <si>
+    <t>10.5.1.84</t>
+  </si>
+  <si>
+    <t>10.5.1.75</t>
+  </si>
+  <si>
+    <t>10.5.1.79</t>
+  </si>
+  <si>
+    <t>10.5.1.83</t>
+  </si>
+  <si>
+    <t>10.5.1.87</t>
+  </si>
+  <si>
+    <t>10.5.1.69</t>
+  </si>
+  <si>
+    <t>10.5.1.73</t>
+  </si>
+  <si>
+    <t>10.5.1.77</t>
+  </si>
+  <si>
+    <t>10.5.1.81</t>
+  </si>
+  <si>
+    <t>10.5.1.85</t>
+  </si>
+  <si>
+    <t>10.5.1.74</t>
+  </si>
+  <si>
+    <t>10.5.1.78</t>
+  </si>
+  <si>
+    <t>10.5.1.82</t>
+  </si>
+  <si>
+    <t>10.5.1.86</t>
+  </si>
+  <si>
+    <t>A1 (H1 - H11)</t>
+  </si>
+  <si>
+    <t>A2 (H1 - H15)</t>
+  </si>
+  <si>
+    <t>A3 (H1 - H30)</t>
+  </si>
+  <si>
+    <t>A4 (H11 - H15)</t>
+  </si>
+  <si>
+    <t>A5 (H11 - H30)</t>
+  </si>
+  <si>
+    <t>A6 (H15 - H30)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="###,###,###,###"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -290,16 +653,54 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor indexed="31"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="31"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -383,6 +784,575 @@
       </right>
       <top/>
       <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="8"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="8"/>
+      </left>
+      <right style="hair">
+        <color indexed="8"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="8"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -392,7 +1362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -427,6 +1397,240 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="51" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="51" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -439,7 +1643,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -725,11 +1929,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IW72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
+    <sheetView zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.28515625" style="1"/>
     <col min="2" max="2" width="18.28515625" style="1"/>
@@ -1865,31 +3067,1861 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IW1"/>
+  <dimension ref="B1:JA46"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="60" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="257" width="13.28515625" style="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="1"/>
+    <col min="11" max="11" width="13.28515625" style="1"/>
+    <col min="12" max="12" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="261" width="13.28515625" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:12" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:12" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B2" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="93" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="93"/>
+      <c r="F2" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="K2" s="94" t="s">
+        <v>113</v>
+      </c>
+      <c r="L2" s="95"/>
+    </row>
+    <row r="3" spans="2:12">
+      <c r="B3" s="40" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="16">
+        <v>2</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="30" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12">
+      <c r="B4" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="74">
+        <v>2</v>
+      </c>
+      <c r="D4" s="75" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="76" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="77" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="77" t="s">
+        <v>188</v>
+      </c>
+      <c r="I4" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="26" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" s="73" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" s="74">
+        <v>2</v>
+      </c>
+      <c r="D5" s="75" t="s">
+        <v>180</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="76" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="77" t="s">
+        <v>184</v>
+      </c>
+      <c r="H5" s="77" t="s">
+        <v>189</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
+      <c r="B6" s="73" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" s="74">
+        <v>2</v>
+      </c>
+      <c r="D6" s="75" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="76" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="77" t="s">
+        <v>185</v>
+      </c>
+      <c r="H6" s="77" t="s">
+        <v>190</v>
+      </c>
+      <c r="I6" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="K6" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="B7" s="73" t="s">
+        <v>178</v>
+      </c>
+      <c r="C7" s="74">
+        <v>2</v>
+      </c>
+      <c r="D7" s="75" t="s">
+        <v>182</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="76" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" s="77" t="s">
+        <v>186</v>
+      </c>
+      <c r="H7" s="77" t="s">
+        <v>191</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="B8" s="73" t="s">
+        <v>179</v>
+      </c>
+      <c r="C8" s="74">
+        <v>2</v>
+      </c>
+      <c r="D8" s="75" t="s">
+        <v>183</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="76" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" s="77" t="s">
+        <v>187</v>
+      </c>
+      <c r="H8" s="77" t="s">
+        <v>192</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="L8" s="26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="15.75" thickBot="1">
+      <c r="B9" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="20">
+        <v>47</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="K9" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="15.75" thickTop="1">
+      <c r="B10" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="20">
+        <v>2</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12">
+      <c r="B11" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="20">
+        <v>9</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12">
+      <c r="B12" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="20">
+        <v>156</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12">
+      <c r="B13" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="20">
+        <v>2</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12">
+      <c r="B14" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="20">
+        <v>2</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="I14" s="25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="B15" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="20">
+        <v>18</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12">
+      <c r="B16" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="20">
+        <v>2</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16">
+      <c r="B17" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="20">
+        <v>13</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16">
+      <c r="B18" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="20">
+        <v>26</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16">
+      <c r="B19" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="20">
+        <v>123</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16">
+      <c r="B20" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="20">
+        <v>131</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" ht="15.75" thickBot="1">
+      <c r="B21" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="42">
+        <v>125</v>
+      </c>
+      <c r="D21" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="G21" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="H21" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="I21" s="44" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" ht="15.75" thickTop="1"/>
+    <row r="23" spans="2:16" ht="15.75" thickBot="1"/>
+    <row r="24" spans="2:16" ht="15.75" thickTop="1">
+      <c r="B24" s="89" t="s">
+        <v>197</v>
+      </c>
+      <c r="C24" s="96"/>
+      <c r="D24" s="90"/>
+      <c r="E24" s="89" t="s">
+        <v>198</v>
+      </c>
+      <c r="F24" s="90"/>
+      <c r="G24" s="89" t="s">
+        <v>199</v>
+      </c>
+      <c r="H24" s="90"/>
+      <c r="I24" s="89" t="s">
+        <v>200</v>
+      </c>
+      <c r="J24" s="90"/>
+      <c r="K24" s="89" t="s">
+        <v>201</v>
+      </c>
+      <c r="L24" s="90"/>
+      <c r="M24" s="89" t="s">
+        <v>202</v>
+      </c>
+      <c r="N24" s="90"/>
+      <c r="O24" s="15"/>
+    </row>
+    <row r="25" spans="2:16">
+      <c r="B25" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="85" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="86"/>
+      <c r="E25" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="G25" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="I25" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="J25" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="K25" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="L25" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="M25" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="N25" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="O25" s="14"/>
+    </row>
+    <row r="26" spans="2:16">
+      <c r="B26" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="85" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="86"/>
+      <c r="E26" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="G26" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="H26" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="I26" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="J26" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="K26" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="L26" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="M26" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="N26" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="O26" s="14"/>
+    </row>
+    <row r="27" spans="2:16">
+      <c r="B27" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="85" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="86"/>
+      <c r="E27" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="G27" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="I27" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="J27" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="K27" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="L27" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="M27" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="N27" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="O27" s="14"/>
+    </row>
+    <row r="28" spans="2:16">
+      <c r="B28" s="31"/>
+      <c r="C28" s="85"/>
+      <c r="D28" s="86"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="66"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="66"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="66"/>
+      <c r="M28" s="31"/>
+      <c r="N28" s="66"/>
+      <c r="O28" s="14"/>
+    </row>
+    <row r="29" spans="2:16">
+      <c r="B29" s="31"/>
+      <c r="C29" s="85"/>
+      <c r="D29" s="86"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="66"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="66"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="66"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="66"/>
+      <c r="O29" s="14"/>
+    </row>
+    <row r="30" spans="2:16" ht="15.75" thickBot="1">
+      <c r="B30" s="33"/>
+      <c r="C30" s="87"/>
+      <c r="D30" s="88"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="67"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="67"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="67"/>
+      <c r="O30" s="14"/>
+    </row>
+    <row r="31" spans="2:16" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B31" s="14"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="14"/>
+    </row>
+    <row r="32" spans="2:16" ht="15.75" thickTop="1">
+      <c r="B32" s="78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="84"/>
+      <c r="D32" s="79"/>
+      <c r="E32" s="78" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="79"/>
+      <c r="G32" s="78" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" s="79"/>
+      <c r="I32" s="89" t="s">
+        <v>14</v>
+      </c>
+      <c r="J32" s="90"/>
+      <c r="K32" s="78" t="s">
+        <v>17</v>
+      </c>
+      <c r="L32" s="79"/>
+      <c r="M32" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="N32" s="79"/>
+      <c r="O32" s="78" t="s">
+        <v>21</v>
+      </c>
+      <c r="P32" s="79"/>
+    </row>
+    <row r="33" spans="2:16">
+      <c r="B33" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="85" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="86"/>
+      <c r="E33" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="G33" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="I33" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="J33" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="K33" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="L33" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="M33" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="N33" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="O33" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="P33" s="66" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16">
+      <c r="B34" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="85" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" s="86"/>
+      <c r="E34" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="G34" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="H34" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="I34" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="J34" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="K34" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="L34" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="M34" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="N34" s="66" t="s">
+        <v>122</v>
+      </c>
+      <c r="O34" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="P34" s="32" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16">
+      <c r="B35" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="85" t="s">
+        <v>146</v>
+      </c>
+      <c r="D35" s="86"/>
+      <c r="E35" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="F35" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="G35" s="31"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="J35" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="K35" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="L35" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="M35" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="N35" s="66" t="s">
+        <v>132</v>
+      </c>
+      <c r="O35" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="P35" s="32" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16">
+      <c r="B36" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="85" t="s">
+        <v>145</v>
+      </c>
+      <c r="D36" s="86"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="66"/>
+      <c r="I36" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="J36" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="K36" s="31"/>
+      <c r="L36" s="66"/>
+      <c r="M36" s="31"/>
+      <c r="N36" s="66"/>
+      <c r="O36" s="31"/>
+      <c r="P36" s="66"/>
+    </row>
+    <row r="37" spans="2:16">
+      <c r="B37" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="85" t="s">
+        <v>147</v>
+      </c>
+      <c r="D37" s="86"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="66"/>
+      <c r="I37" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="J37" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="K37" s="31"/>
+      <c r="L37" s="66"/>
+      <c r="M37" s="31"/>
+      <c r="N37" s="66"/>
+      <c r="O37" s="31"/>
+      <c r="P37" s="66"/>
+    </row>
+    <row r="38" spans="2:16" ht="15.75" thickBot="1">
+      <c r="B38" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" s="87" t="s">
+        <v>148</v>
+      </c>
+      <c r="D38" s="88"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="67"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="67"/>
+      <c r="K38" s="33"/>
+      <c r="L38" s="67"/>
+      <c r="M38" s="33"/>
+      <c r="N38" s="67"/>
+      <c r="O38" s="33"/>
+      <c r="P38" s="67"/>
+    </row>
+    <row r="39" spans="2:16" ht="16.5" thickTop="1" thickBot="1"/>
+    <row r="40" spans="2:16">
+      <c r="B40" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="98"/>
+      <c r="D40" s="92"/>
+      <c r="E40" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="F40" s="92"/>
+      <c r="G40" s="91" t="s">
+        <v>26</v>
+      </c>
+      <c r="H40" s="92"/>
+      <c r="I40" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="J40" s="92"/>
+      <c r="K40" s="91" t="s">
+        <v>29</v>
+      </c>
+      <c r="L40" s="92"/>
+      <c r="M40" s="91" t="s">
+        <v>31</v>
+      </c>
+      <c r="N40" s="92"/>
+    </row>
+    <row r="41" spans="2:16">
+      <c r="B41" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="85" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="97"/>
+      <c r="E41" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="F41" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="G41" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="H41" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="I41" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="J41" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="K41" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="L41" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="M41" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="N41" s="68" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16">
+      <c r="B42" s="69" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="85" t="s">
+        <v>124</v>
+      </c>
+      <c r="D42" s="97"/>
+      <c r="E42" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="G42" s="69" t="s">
+        <v>57</v>
+      </c>
+      <c r="H42" s="71" t="s">
+        <v>125</v>
+      </c>
+      <c r="I42" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="J42" s="71" t="s">
+        <v>126</v>
+      </c>
+      <c r="K42" s="69" t="s">
+        <v>57</v>
+      </c>
+      <c r="L42" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="M42" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="N42" s="71" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16">
+      <c r="B43" s="69" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="85" t="s">
+        <v>134</v>
+      </c>
+      <c r="D43" s="97"/>
+      <c r="E43" s="69" t="s">
+        <v>65</v>
+      </c>
+      <c r="F43" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="G43" s="69" t="s">
+        <v>61</v>
+      </c>
+      <c r="H43" s="71" t="s">
+        <v>150</v>
+      </c>
+      <c r="I43" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="J43" s="71" t="s">
+        <v>153</v>
+      </c>
+      <c r="K43" s="69" t="s">
+        <v>66</v>
+      </c>
+      <c r="L43" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="M43" s="69" t="s">
+        <v>141</v>
+      </c>
+      <c r="N43" s="71" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16">
+      <c r="B44" s="69"/>
+      <c r="C44" s="80"/>
+      <c r="D44" s="81"/>
+      <c r="E44" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="F44" s="71" t="s">
+        <v>54</v>
+      </c>
+      <c r="G44" s="69" t="s">
+        <v>66</v>
+      </c>
+      <c r="H44" s="71" t="s">
+        <v>152</v>
+      </c>
+      <c r="I44" s="69" t="s">
+        <v>65</v>
+      </c>
+      <c r="J44" s="71" t="s">
+        <v>154</v>
+      </c>
+      <c r="K44" s="69" t="s">
+        <v>143</v>
+      </c>
+      <c r="L44" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="M44" s="69"/>
+      <c r="N44" s="71"/>
+    </row>
+    <row r="45" spans="2:16">
+      <c r="B45" s="69"/>
+      <c r="C45" s="80"/>
+      <c r="D45" s="81"/>
+      <c r="E45" s="69" t="s">
+        <v>141</v>
+      </c>
+      <c r="F45" s="71" t="s">
+        <v>42</v>
+      </c>
+      <c r="G45" s="69" t="s">
+        <v>144</v>
+      </c>
+      <c r="H45" s="71" t="s">
+        <v>151</v>
+      </c>
+      <c r="I45" s="69"/>
+      <c r="J45" s="71"/>
+      <c r="K45" s="69"/>
+      <c r="L45" s="71"/>
+      <c r="M45" s="69"/>
+      <c r="N45" s="71"/>
+    </row>
+    <row r="46" spans="2:16" ht="15.75" thickBot="1">
+      <c r="B46" s="70"/>
+      <c r="C46" s="82"/>
+      <c r="D46" s="83"/>
+      <c r="E46" s="70" t="s">
+        <v>142</v>
+      </c>
+      <c r="F46" s="72" t="s">
+        <v>44</v>
+      </c>
+      <c r="G46" s="70"/>
+      <c r="H46" s="72"/>
+      <c r="I46" s="70"/>
+      <c r="J46" s="72"/>
+      <c r="K46" s="70"/>
+      <c r="L46" s="72"/>
+      <c r="M46" s="70"/>
+      <c r="N46" s="72"/>
+    </row>
+  </sheetData>
+  <mergeCells count="39">
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="K40:L40"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IW1"/>
+  <dimension ref="A2:IW38"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="257" width="13.28515625" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:15">
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="55" t="s">
+        <v>157</v>
+      </c>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+    </row>
+    <row r="3" spans="2:15">
+      <c r="B3" s="99" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="101"/>
+      <c r="G3" s="99" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="58"/>
+    </row>
+    <row r="4" spans="2:15">
+      <c r="B4" s="102"/>
+      <c r="C4" s="103"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="104"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="104"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="61"/>
+    </row>
+    <row r="5" spans="2:15">
+      <c r="B5" s="102"/>
+      <c r="C5" s="103"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="104"/>
+      <c r="G5" s="102"/>
+      <c r="H5" s="103"/>
+      <c r="I5" s="103"/>
+      <c r="J5" s="104"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="60"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="61"/>
+    </row>
+    <row r="6" spans="2:15">
+      <c r="B6" s="102"/>
+      <c r="C6" s="103"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="104"/>
+      <c r="G6" s="102"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="103"/>
+      <c r="J6" s="104"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="61"/>
+    </row>
+    <row r="7" spans="2:15">
+      <c r="B7" s="102"/>
+      <c r="C7" s="103"/>
+      <c r="D7" s="103"/>
+      <c r="E7" s="104"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="103"/>
+      <c r="J7" s="104"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="60"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="61"/>
+    </row>
+    <row r="8" spans="2:15">
+      <c r="B8" s="102"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="104"/>
+      <c r="G8" s="102"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="103"/>
+      <c r="J8" s="104"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="59"/>
+      <c r="M8" s="60"/>
+      <c r="N8" s="60"/>
+      <c r="O8" s="61"/>
+    </row>
+    <row r="9" spans="2:15">
+      <c r="B9" s="102"/>
+      <c r="C9" s="103"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="104"/>
+      <c r="G9" s="102"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="103"/>
+      <c r="J9" s="104"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="59"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="60"/>
+      <c r="O9" s="61"/>
+    </row>
+    <row r="10" spans="2:15">
+      <c r="B10" s="102"/>
+      <c r="C10" s="103"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="104"/>
+      <c r="G10" s="102"/>
+      <c r="H10" s="103"/>
+      <c r="I10" s="103"/>
+      <c r="J10" s="104"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="59"/>
+      <c r="M10" s="60"/>
+      <c r="N10" s="60"/>
+      <c r="O10" s="61"/>
+    </row>
+    <row r="11" spans="2:15">
+      <c r="B11" s="102"/>
+      <c r="C11" s="103"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="104"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="103"/>
+      <c r="I11" s="103"/>
+      <c r="J11" s="104"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="59"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="60"/>
+      <c r="O11" s="61"/>
+    </row>
+    <row r="12" spans="2:15">
+      <c r="B12" s="102"/>
+      <c r="C12" s="103"/>
+      <c r="D12" s="103"/>
+      <c r="E12" s="104"/>
+      <c r="G12" s="102"/>
+      <c r="H12" s="103"/>
+      <c r="I12" s="103"/>
+      <c r="J12" s="104"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="59"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="60"/>
+      <c r="O12" s="61"/>
+    </row>
+    <row r="13" spans="2:15">
+      <c r="B13" s="102"/>
+      <c r="C13" s="103"/>
+      <c r="D13" s="103"/>
+      <c r="E13" s="104"/>
+      <c r="G13" s="102"/>
+      <c r="H13" s="103"/>
+      <c r="I13" s="103"/>
+      <c r="J13" s="104"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="59"/>
+      <c r="M13" s="60"/>
+      <c r="N13" s="60"/>
+      <c r="O13" s="61"/>
+    </row>
+    <row r="14" spans="2:15">
+      <c r="B14" s="102"/>
+      <c r="C14" s="103"/>
+      <c r="D14" s="103"/>
+      <c r="E14" s="104"/>
+      <c r="G14" s="102"/>
+      <c r="H14" s="103"/>
+      <c r="I14" s="103"/>
+      <c r="J14" s="104"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="59"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="60"/>
+      <c r="O14" s="61"/>
+    </row>
+    <row r="15" spans="2:15">
+      <c r="B15" s="102"/>
+      <c r="C15" s="103"/>
+      <c r="D15" s="103"/>
+      <c r="E15" s="104"/>
+      <c r="G15" s="102"/>
+      <c r="H15" s="103"/>
+      <c r="I15" s="103"/>
+      <c r="J15" s="104"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="59"/>
+      <c r="M15" s="60"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="61"/>
+    </row>
+    <row r="16" spans="2:15">
+      <c r="B16" s="102"/>
+      <c r="C16" s="103"/>
+      <c r="D16" s="103"/>
+      <c r="E16" s="104"/>
+      <c r="G16" s="102"/>
+      <c r="H16" s="103"/>
+      <c r="I16" s="103"/>
+      <c r="J16" s="104"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="59"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="60"/>
+      <c r="O16" s="61"/>
+    </row>
+    <row r="17" spans="2:15">
+      <c r="B17" s="102"/>
+      <c r="C17" s="103"/>
+      <c r="D17" s="103"/>
+      <c r="E17" s="104"/>
+      <c r="G17" s="102"/>
+      <c r="H17" s="103"/>
+      <c r="I17" s="103"/>
+      <c r="J17" s="104"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="59"/>
+      <c r="M17" s="60"/>
+      <c r="N17" s="60"/>
+      <c r="O17" s="61"/>
+    </row>
+    <row r="18" spans="2:15">
+      <c r="B18" s="105"/>
+      <c r="C18" s="106"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="107"/>
+      <c r="G18" s="105"/>
+      <c r="H18" s="106"/>
+      <c r="I18" s="106"/>
+      <c r="J18" s="107"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="62"/>
+      <c r="M18" s="63"/>
+      <c r="N18" s="64" t="s">
+        <v>17</v>
+      </c>
+      <c r="O18" s="64" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15">
+      <c r="B22" t="s">
+        <v>155</v>
+      </c>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="G22" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="M22" s="60"/>
+      <c r="N22" s="60"/>
+      <c r="O22" s="60"/>
+    </row>
+    <row r="23" spans="2:15">
+      <c r="B23" s="45"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="47"/>
+      <c r="G23" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" s="100"/>
+      <c r="I23" s="100"/>
+      <c r="J23" s="101"/>
+      <c r="K23" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="L23" s="99" t="s">
+        <v>6</v>
+      </c>
+      <c r="M23" s="100"/>
+      <c r="N23" s="100"/>
+      <c r="O23" s="101"/>
+    </row>
+    <row r="24" spans="2:15">
+      <c r="B24" s="48"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="50"/>
+      <c r="G24" s="102"/>
+      <c r="H24" s="103"/>
+      <c r="I24" s="103"/>
+      <c r="J24" s="104"/>
+      <c r="K24" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="L24" s="102"/>
+      <c r="M24" s="103"/>
+      <c r="N24" s="103"/>
+      <c r="O24" s="104"/>
+    </row>
+    <row r="25" spans="2:15">
+      <c r="B25" s="48"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="50"/>
+      <c r="G25" s="102"/>
+      <c r="H25" s="103"/>
+      <c r="I25" s="103"/>
+      <c r="J25" s="104"/>
+      <c r="K25" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="L25" s="102"/>
+      <c r="M25" s="103"/>
+      <c r="N25" s="103"/>
+      <c r="O25" s="104"/>
+    </row>
+    <row r="26" spans="2:15">
+      <c r="B26" s="51"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="53"/>
+      <c r="G26" s="102"/>
+      <c r="H26" s="103"/>
+      <c r="I26" s="103"/>
+      <c r="J26" s="104"/>
+      <c r="K26" s="54" t="s">
+        <v>161</v>
+      </c>
+      <c r="L26" s="105"/>
+      <c r="M26" s="106"/>
+      <c r="N26" s="106"/>
+      <c r="O26" s="107"/>
+    </row>
+    <row r="27" spans="2:15">
+      <c r="G27" s="102"/>
+      <c r="H27" s="103"/>
+      <c r="I27" s="103"/>
+      <c r="J27" s="104"/>
+      <c r="K27" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="L27" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="M27" s="100"/>
+      <c r="N27" s="100"/>
+      <c r="O27" s="101"/>
+    </row>
+    <row r="28" spans="2:15">
+      <c r="G28" s="102"/>
+      <c r="H28" s="103"/>
+      <c r="I28" s="103"/>
+      <c r="J28" s="104"/>
+      <c r="K28" s="54" t="s">
+        <v>163</v>
+      </c>
+      <c r="L28" s="105"/>
+      <c r="M28" s="106"/>
+      <c r="N28" s="106"/>
+      <c r="O28" s="107"/>
+    </row>
+    <row r="29" spans="2:15">
+      <c r="G29" s="102"/>
+      <c r="H29" s="103"/>
+      <c r="I29" s="103"/>
+      <c r="J29" s="104"/>
+      <c r="K29" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="L29" s="108" t="s">
+        <v>21</v>
+      </c>
+      <c r="M29" s="109"/>
+      <c r="N29" s="109"/>
+      <c r="O29" s="110"/>
+    </row>
+    <row r="30" spans="2:15">
+      <c r="G30" s="105"/>
+      <c r="H30" s="106"/>
+      <c r="I30" s="106"/>
+      <c r="J30" s="107"/>
+      <c r="K30" s="54" t="s">
+        <v>165</v>
+      </c>
+      <c r="L30" s="59"/>
+      <c r="M30" s="60"/>
+      <c r="N30" s="60"/>
+      <c r="O30" s="61"/>
+    </row>
+    <row r="31" spans="2:15">
+      <c r="B31" s="49" t="s">
+        <v>156</v>
+      </c>
+      <c r="G31" s="99" t="s">
+        <v>31</v>
+      </c>
+      <c r="H31" s="100"/>
+      <c r="I31" s="100"/>
+      <c r="J31" s="101"/>
+      <c r="K31" s="54" t="s">
+        <v>166</v>
+      </c>
+      <c r="L31" s="108" t="s">
+        <v>24</v>
+      </c>
+      <c r="M31" s="109"/>
+      <c r="N31" s="109"/>
+      <c r="O31" s="110"/>
+    </row>
+    <row r="32" spans="2:15">
+      <c r="G32" s="102"/>
+      <c r="H32" s="103"/>
+      <c r="I32" s="103"/>
+      <c r="J32" s="104"/>
+      <c r="K32" s="54" t="s">
+        <v>167</v>
+      </c>
+      <c r="L32" s="108" t="s">
+        <v>12</v>
+      </c>
+      <c r="M32" s="109"/>
+      <c r="N32" s="109"/>
+      <c r="O32" s="110"/>
+    </row>
+    <row r="33" spans="7:15">
+      <c r="G33" s="102"/>
+      <c r="H33" s="103"/>
+      <c r="I33" s="103"/>
+      <c r="J33" s="104"/>
+      <c r="K33" s="54" t="s">
+        <v>168</v>
+      </c>
+      <c r="L33" s="59"/>
+      <c r="M33" s="60"/>
+      <c r="N33" s="60"/>
+      <c r="O33" s="61"/>
+    </row>
+    <row r="34" spans="7:15">
+      <c r="G34" s="102"/>
+      <c r="H34" s="103"/>
+      <c r="I34" s="103"/>
+      <c r="J34" s="104"/>
+      <c r="K34" s="54" t="s">
+        <v>169</v>
+      </c>
+      <c r="L34" s="59"/>
+      <c r="M34" s="60"/>
+      <c r="N34" s="60"/>
+      <c r="O34" s="61"/>
+    </row>
+    <row r="35" spans="7:15">
+      <c r="G35" s="102"/>
+      <c r="H35" s="103"/>
+      <c r="I35" s="103"/>
+      <c r="J35" s="104"/>
+      <c r="K35" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="L35" s="59"/>
+      <c r="M35" s="60"/>
+      <c r="N35" s="60"/>
+      <c r="O35" s="61"/>
+    </row>
+    <row r="36" spans="7:15">
+      <c r="G36" s="102"/>
+      <c r="H36" s="103"/>
+      <c r="I36" s="103"/>
+      <c r="J36" s="104"/>
+      <c r="K36" s="54" t="s">
+        <v>171</v>
+      </c>
+      <c r="L36" s="59"/>
+      <c r="M36" s="60"/>
+      <c r="N36" s="60"/>
+      <c r="O36" s="61"/>
+    </row>
+    <row r="37" spans="7:15">
+      <c r="G37" s="102"/>
+      <c r="H37" s="103"/>
+      <c r="I37" s="103"/>
+      <c r="J37" s="104"/>
+      <c r="K37" s="54" t="s">
+        <v>172</v>
+      </c>
+      <c r="L37" s="59"/>
+      <c r="M37" s="60"/>
+      <c r="N37" s="60"/>
+      <c r="O37" s="61"/>
+    </row>
+    <row r="38" spans="7:15">
+      <c r="G38" s="105"/>
+      <c r="H38" s="106"/>
+      <c r="I38" s="106"/>
+      <c r="J38" s="107"/>
+      <c r="K38" s="54" t="s">
+        <v>173</v>
+      </c>
+      <c r="L38" s="62"/>
+      <c r="M38" s="63"/>
+      <c r="N38" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="O38" s="65" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B3:E18"/>
+    <mergeCell ref="G3:J18"/>
+    <mergeCell ref="G31:J38"/>
+    <mergeCell ref="G23:J30"/>
+    <mergeCell ref="L23:O26"/>
+    <mergeCell ref="L27:O28"/>
+    <mergeCell ref="L29:O29"/>
+    <mergeCell ref="L31:O31"/>
+    <mergeCell ref="L32:O32"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>